<commit_message>
test plan updated 1.0.1
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
   <si>
     <t>project name</t>
   </si>
@@ -315,12 +315,41 @@
   <si>
     <t>after click on continue button, user wil be in reg page. An alert message will be open just below the menu bar. The text is ' Warning: You must agree to the Privacy Policy!'</t>
   </si>
+  <si>
+    <t xml:space="preserve">verifying User is in download page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that User has come in download page </t>
+  </si>
+  <si>
+    <t>provide valid email and password
+for user login</t>
+  </si>
+  <si>
+    <t>1. open "https://demo.opencart.com/" page in browser.
+2. click on my account tab,dropdown list will be open
+3. now click on login from dropdown list. Login page will be open
+4. login user account. User account home page will be open
+5. now click on downloads button from this page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after click on downloads button, user will be in downloads page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user has been in downloads page </t>
+  </si>
+  <si>
+    <t>16/02/2020</t>
+  </si>
+  <si>
+    <t>user account home page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +373,14 @@
     <font>
       <b/>
       <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -382,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -423,6 +460,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,14 +773,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" customWidth="1"/>
     <col min="5" max="5" width="38.85546875" customWidth="1"/>
@@ -1287,22 +1330,52 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="12"/>
+    <row r="16" spans="1:17" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>3</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="5">
+        <v>91703</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>

</xml_diff>